<commit_message>
added funcionality to read excel files
</commit_message>
<xml_diff>
--- a/FRJ.Tools.SimpleWorkSheet.Examples/Output/01_HelloWorld.xlsx
+++ b/FRJ.Tools.SimpleWorkSheet.Examples/Output/01_HelloWorld.xlsx
@@ -5,7 +5,7 @@
     <x:workbookView/>
   </x:bookViews>
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HelloWorld" sheetId="1" r:id="R690bf4fdc887430a"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="HelloWorld" sheetId="1" r:id="Rca65a656379b41b5"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -27,7 +27,7 @@
     <x:font/>
     <x:font>
       <x:sz val="12"/>
-      <x:color rgb="000000"/>
+      <x:color rgb="FF000000"/>
       <x:name val="Aptos Narrow"/>
     </x:font>
   </x:fonts>

</xml_diff>